<commit_message>
Adding mobile barcode scanning
</commit_message>
<xml_diff>
--- a/server/uploads/images/template.xlsx
+++ b/server/uploads/images/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\library_management_system\server\uploads\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
   <si>
     <t>title</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Erdoglija, Kragujevac</t>
+  </si>
+  <si>
+    <t>barcode</t>
   </si>
 </sst>
 </file>
@@ -544,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,13 +561,13 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,19 +590,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -619,21 +625,22 @@
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -653,21 +660,22 @@
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -687,21 +695,22 @@
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -721,21 +730,22 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -755,21 +765,22 @@
       <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -789,21 +800,22 @@
       <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -823,21 +835,22 @@
       <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -857,21 +870,22 @@
       <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -891,21 +905,22 @@
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -925,21 +940,22 @@
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -959,21 +975,22 @@
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -993,21 +1010,22 @@
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -1027,19 +1045,20 @@
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding readme and some additional changes
</commit_message>
<xml_diff>
--- a/server/uploads/images/template.xlsx
+++ b/server/uploads/images/template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="89">
   <si>
     <t>title</t>
   </si>
@@ -199,13 +199,112 @@
   </si>
   <si>
     <t>barcode</t>
+  </si>
+  <si>
+    <t>Kros</t>
+  </si>
+  <si>
+    <t>64647320e5aef707a57f4cc0</t>
+  </si>
+  <si>
+    <t>Džejms Paterson</t>
+  </si>
+  <si>
+    <t>Dvostruka prevara</t>
+  </si>
+  <si>
+    <t>Dani lova</t>
+  </si>
+  <si>
+    <t>Suđenje</t>
+  </si>
+  <si>
+    <t>Ja, Aleks Kros</t>
+  </si>
+  <si>
+    <t>Unakrsna vatra</t>
+  </si>
+  <si>
+    <t>Beži, Krose</t>
+  </si>
+  <si>
+    <t>Tako mi svega</t>
+  </si>
+  <si>
+    <t>Po cenu života</t>
+  </si>
+  <si>
+    <t>Prikrade se pauk</t>
+  </si>
+  <si>
+    <t>Ubistvo u Orijent Ekspresu</t>
+  </si>
+  <si>
+    <t>roman</t>
+  </si>
+  <si>
+    <t>646473ace5aef707a57f4cc4</t>
+  </si>
+  <si>
+    <t>Agata Kristi</t>
+  </si>
+  <si>
+    <t>ABC ubistva</t>
+  </si>
+  <si>
+    <t>Stanica Padington</t>
+  </si>
+  <si>
+    <t>krimi, roman</t>
+  </si>
+  <si>
+    <t>engleski</t>
+  </si>
+  <si>
+    <t>Tajanstveni slučaj u Stajlsu</t>
+  </si>
+  <si>
+    <t>Orlovi rano lete</t>
+  </si>
+  <si>
+    <t>6464740fe5aef707a57f4cc6</t>
+  </si>
+  <si>
+    <t>Branko Ćopić</t>
+  </si>
+  <si>
+    <t>Bašta sljezove boje</t>
+  </si>
+  <si>
+    <t>zbirka priča</t>
+  </si>
+  <si>
+    <t>Ježeva kućica</t>
+  </si>
+  <si>
+    <t>basna</t>
+  </si>
+  <si>
+    <t>hrvatski</t>
+  </si>
+  <si>
+    <t>Klub za vešanje</t>
+  </si>
+  <si>
+    <t>64d3f2f20038c30c545d2cbb</t>
+  </si>
+  <si>
+    <t>Toni Parsons</t>
+  </si>
+  <si>
+    <t>Jedan po jedan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +332,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -251,25 +357,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -547,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,6 +670,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
@@ -612,7 +722,7 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -625,14 +735,16 @@
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="6">
+        <v>9781551923708</v>
+      </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -647,7 +759,7 @@
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -660,14 +772,16 @@
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="6">
+        <v>9780671027582</v>
+      </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -682,7 +796,7 @@
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -695,14 +809,16 @@
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="6">
+        <v>9780061120084</v>
+      </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>49</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -717,7 +833,7 @@
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -730,14 +846,16 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="6">
+        <v>9780446310789</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>49</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -752,7 +870,7 @@
       <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -765,14 +883,16 @@
       <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="6">
+        <v>9780141439617</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>49</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -787,7 +907,7 @@
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -800,14 +920,16 @@
       <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="6">
+        <v>9781400079276</v>
+      </c>
       <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -822,7 +944,7 @@
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -835,14 +957,16 @@
       <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="6">
+        <v>9780743273565</v>
+      </c>
       <c r="I8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -857,7 +981,7 @@
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -870,14 +994,16 @@
       <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="6">
+        <v>9780385484510</v>
+      </c>
       <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -892,7 +1018,7 @@
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -905,14 +1031,16 @@
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="6">
+        <v>9780679745203</v>
+      </c>
       <c r="I10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="L10" s="2" t="s">
@@ -927,7 +1055,7 @@
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -940,14 +1068,16 @@
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="6">
+        <v>9780061122415</v>
+      </c>
       <c r="I11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="3" t="s">
         <v>51</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -962,7 +1092,7 @@
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -975,14 +1105,16 @@
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="6">
+        <v>9780671003753</v>
+      </c>
       <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="L12" s="2" t="s">
@@ -997,7 +1129,7 @@
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1010,14 +1142,16 @@
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="6">
+        <v>9780553280360</v>
+      </c>
       <c r="I13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="3" t="s">
         <v>51</v>
       </c>
       <c r="L13" s="2" t="s">
@@ -1032,7 +1166,7 @@
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1045,20 +1179,706 @@
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="6">
+        <v>9780142004231</v>
+      </c>
       <c r="I14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>51</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>54</v>
       </c>
       <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2003</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="6">
+        <v>9781400043635</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2004</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="6">
+        <v>9780743227445</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2006</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="6">
+        <v>9780385490817</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2007</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="6">
+        <v>9780679764020</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2008</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="6">
+        <v>9780061125379</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2010</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="6">
+        <v>9780451169535</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2011</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="6">
+        <v>9780142001742</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="6">
+        <v>9781400043192</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="6">
+        <v>9780743273565</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="6">
+        <v>9780385511611</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="6">
+        <v>9780679768356</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="6">
+        <v>9780061125348</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="6">
+        <v>9780451191147</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2013</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="6">
+        <v>9780142004231</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="6">
+        <v>9781400043635</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="6">
+        <v>9780743227445</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="6">
+        <v>9780385490817</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="6">
+        <v>9780679764020</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="6">
+        <v>9780061125379</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>